<commit_message>
Significant development work in SAR and Budget cleaning and processing in support of International Joint Development and PBL.
I'm about to change how I handle the RawHeaderList.csv and wanted to commit first.
</commit_message>
<xml_diff>
--- a/FOIA SAR data/JSF/2015-12 JSF SAR DataDraw.xlsx
+++ b/FOIA SAR data/JSF/2015-12 JSF SAR DataDraw.xlsx
@@ -2,21 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\2015-09 Joint Development\Research\JSF F-35\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\2007-01 PROFESSIONAL SERVICES\R scripts and data\FOIA SAR data\JSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10095" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10095" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CostSummary" sheetId="1" r:id="rId1"/>
     <sheet name="Funding Summary" sheetId="2" r:id="rId2"/>
     <sheet name="Low Rate Initial Production" sheetId="3" r:id="rId3"/>
     <sheet name="Foreign Military Sales" sheetId="4" r:id="rId4"/>
-    <sheet name="Unit Cost " sheetId="5" r:id="rId5"/>
+    <sheet name="Unit Cost" sheetId="5" r:id="rId5"/>
     <sheet name="Cost Variance" sheetId="6" r:id="rId6"/>
     <sheet name="Contracts " sheetId="7" r:id="rId7"/>
     <sheet name="Deliveries and Expenditures" sheetId="8" r:id="rId8"/>
@@ -1349,7 +1349,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1943,25 +1943,31 @@
     <xf numFmtId="10" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1989,6 +1995,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2023,21 +2038,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="7"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2382,76 +2382,76 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="102"/>
-      <c r="B3" s="109" t="s">
+      <c r="A3" s="109"/>
+      <c r="B3" s="111" t="s">
         <v>149</v>
       </c>
-      <c r="C3" s="110"/>
+      <c r="C3" s="112"/>
       <c r="D3" s="29"/>
       <c r="E3" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="F3" s="109" t="s">
+      <c r="F3" s="111" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="110"/>
-      <c r="H3" s="113"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="115"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="103"/>
-      <c r="B4" s="111"/>
-      <c r="C4" s="112"/>
+      <c r="A4" s="110"/>
+      <c r="B4" s="113"/>
+      <c r="C4" s="114"/>
       <c r="D4" s="30"/>
       <c r="E4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="114"/>
-      <c r="G4" s="115"/>
-      <c r="H4" s="116"/>
+      <c r="F4" s="116"/>
+      <c r="G4" s="117"/>
+      <c r="H4" s="118"/>
     </row>
     <row r="5" spans="1:10" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="104" t="s">
+      <c r="A5" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="104" t="s">
+      <c r="B5" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="109" t="s">
+      <c r="C5" s="111" t="s">
         <v>184</v>
       </c>
-      <c r="D5" s="113"/>
-      <c r="E5" s="104" t="s">
+      <c r="D5" s="115"/>
+      <c r="E5" s="107" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="111"/>
-      <c r="G5" s="112"/>
-      <c r="H5" s="117"/>
+      <c r="F5" s="113"/>
+      <c r="G5" s="114"/>
+      <c r="H5" s="119"/>
     </row>
     <row r="6" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="107"/>
-      <c r="B6" s="105"/>
-      <c r="C6" s="114"/>
-      <c r="D6" s="116"/>
-      <c r="E6" s="107"/>
-      <c r="F6" s="104" t="s">
+      <c r="A6" s="120"/>
+      <c r="B6" s="122"/>
+      <c r="C6" s="116"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="120"/>
+      <c r="F6" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="104" t="s">
+      <c r="G6" s="107" t="s">
         <v>185</v>
       </c>
-      <c r="H6" s="104" t="s">
+      <c r="H6" s="107" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="108"/>
-      <c r="B7" s="106"/>
-      <c r="C7" s="111"/>
-      <c r="D7" s="117"/>
-      <c r="E7" s="108"/>
-      <c r="F7" s="108"/>
-      <c r="G7" s="108"/>
-      <c r="H7" s="108"/>
+      <c r="A7" s="121"/>
+      <c r="B7" s="108"/>
+      <c r="C7" s="113"/>
+      <c r="D7" s="119"/>
+      <c r="E7" s="121"/>
+      <c r="F7" s="121"/>
+      <c r="G7" s="121"/>
+      <c r="H7" s="121"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
@@ -2758,76 +2758,76 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="102"/>
-      <c r="B21" s="109" t="s">
+      <c r="A21" s="109"/>
+      <c r="B21" s="111" t="s">
         <v>149</v>
       </c>
-      <c r="C21" s="110"/>
+      <c r="C21" s="112"/>
       <c r="D21" s="29"/>
       <c r="E21" s="69" t="s">
         <v>150</v>
       </c>
-      <c r="F21" s="109" t="s">
+      <c r="F21" s="111" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="110"/>
-      <c r="H21" s="113"/>
+      <c r="G21" s="112"/>
+      <c r="H21" s="115"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="103"/>
-      <c r="B22" s="111"/>
-      <c r="C22" s="112"/>
+      <c r="A22" s="110"/>
+      <c r="B22" s="113"/>
+      <c r="C22" s="114"/>
       <c r="D22" s="70"/>
       <c r="E22" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="F22" s="114"/>
-      <c r="G22" s="115"/>
-      <c r="H22" s="116"/>
+      <c r="F22" s="116"/>
+      <c r="G22" s="117"/>
+      <c r="H22" s="118"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="104" t="s">
+      <c r="A23" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="104" t="s">
+      <c r="B23" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="109" t="s">
+      <c r="C23" s="111" t="s">
         <v>184</v>
       </c>
-      <c r="D23" s="113"/>
-      <c r="E23" s="104" t="s">
+      <c r="D23" s="115"/>
+      <c r="E23" s="107" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="111"/>
-      <c r="G23" s="112"/>
-      <c r="H23" s="117"/>
+      <c r="F23" s="113"/>
+      <c r="G23" s="114"/>
+      <c r="H23" s="119"/>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="107"/>
-      <c r="B24" s="105"/>
-      <c r="C24" s="114"/>
-      <c r="D24" s="116"/>
-      <c r="E24" s="107"/>
-      <c r="F24" s="104" t="s">
+      <c r="A24" s="120"/>
+      <c r="B24" s="122"/>
+      <c r="C24" s="116"/>
+      <c r="D24" s="118"/>
+      <c r="E24" s="120"/>
+      <c r="F24" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="G24" s="104" t="s">
+      <c r="G24" s="107" t="s">
         <v>185</v>
       </c>
-      <c r="H24" s="104" t="s">
+      <c r="H24" s="107" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="108"/>
-      <c r="B25" s="106"/>
-      <c r="C25" s="111"/>
-      <c r="D25" s="117"/>
-      <c r="E25" s="108"/>
-      <c r="F25" s="108"/>
-      <c r="G25" s="108"/>
-      <c r="H25" s="108"/>
+      <c r="A25" s="121"/>
+      <c r="B25" s="108"/>
+      <c r="C25" s="113"/>
+      <c r="D25" s="119"/>
+      <c r="E25" s="121"/>
+      <c r="F25" s="121"/>
+      <c r="G25" s="121"/>
+      <c r="H25" s="121"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
@@ -3130,10 +3130,10 @@
       <c r="B38" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="104" t="s">
+      <c r="C38" s="107" t="s">
         <v>152</v>
       </c>
-      <c r="D38" s="104" t="s">
+      <c r="D38" s="107" t="s">
         <v>16</v>
       </c>
     </row>
@@ -3144,8 +3144,8 @@
       <c r="B39" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="106"/>
-      <c r="D39" s="106"/>
+      <c r="C39" s="108"/>
+      <c r="D39" s="108"/>
     </row>
     <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
@@ -3195,76 +3195,76 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="102"/>
-      <c r="B45" s="109" t="s">
+      <c r="A45" s="109"/>
+      <c r="B45" s="111" t="s">
         <v>149</v>
       </c>
-      <c r="C45" s="110"/>
+      <c r="C45" s="112"/>
       <c r="D45" s="29"/>
       <c r="E45" s="69" t="s">
         <v>150</v>
       </c>
-      <c r="F45" s="109" t="s">
+      <c r="F45" s="111" t="s">
         <v>15</v>
       </c>
-      <c r="G45" s="110"/>
-      <c r="H45" s="113"/>
+      <c r="G45" s="112"/>
+      <c r="H45" s="115"/>
     </row>
     <row r="46" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="103"/>
-      <c r="B46" s="111"/>
-      <c r="C46" s="112"/>
+      <c r="A46" s="110"/>
+      <c r="B46" s="113"/>
+      <c r="C46" s="114"/>
       <c r="D46" s="70"/>
       <c r="E46" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="F46" s="114"/>
-      <c r="G46" s="115"/>
-      <c r="H46" s="116"/>
+      <c r="F46" s="116"/>
+      <c r="G46" s="117"/>
+      <c r="H46" s="118"/>
     </row>
     <row r="47" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="104" t="s">
+      <c r="A47" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="104" t="s">
+      <c r="B47" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="C47" s="109" t="s">
+      <c r="C47" s="111" t="s">
         <v>184</v>
       </c>
-      <c r="D47" s="113"/>
-      <c r="E47" s="104" t="s">
+      <c r="D47" s="115"/>
+      <c r="E47" s="107" t="s">
         <v>16</v>
       </c>
-      <c r="F47" s="111"/>
-      <c r="G47" s="112"/>
-      <c r="H47" s="117"/>
+      <c r="F47" s="113"/>
+      <c r="G47" s="114"/>
+      <c r="H47" s="119"/>
     </row>
     <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="107"/>
-      <c r="B48" s="105"/>
-      <c r="C48" s="114"/>
-      <c r="D48" s="116"/>
-      <c r="E48" s="107"/>
-      <c r="F48" s="104" t="s">
+      <c r="A48" s="120"/>
+      <c r="B48" s="122"/>
+      <c r="C48" s="116"/>
+      <c r="D48" s="118"/>
+      <c r="E48" s="120"/>
+      <c r="F48" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="G48" s="104" t="s">
+      <c r="G48" s="107" t="s">
         <v>185</v>
       </c>
-      <c r="H48" s="104" t="s">
+      <c r="H48" s="107" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="108"/>
-      <c r="B49" s="106"/>
-      <c r="C49" s="111"/>
-      <c r="D49" s="117"/>
-      <c r="E49" s="108"/>
-      <c r="F49" s="108"/>
-      <c r="G49" s="108"/>
-      <c r="H49" s="108"/>
+      <c r="A49" s="121"/>
+      <c r="B49" s="108"/>
+      <c r="C49" s="113"/>
+      <c r="D49" s="119"/>
+      <c r="E49" s="121"/>
+      <c r="F49" s="121"/>
+      <c r="G49" s="121"/>
+      <c r="H49" s="121"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="15" t="s">
@@ -3558,10 +3558,10 @@
       <c r="B62" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C62" s="104" t="s">
+      <c r="C62" s="107" t="s">
         <v>152</v>
       </c>
-      <c r="D62" s="104" t="s">
+      <c r="D62" s="107" t="s">
         <v>16</v>
       </c>
     </row>
@@ -3572,8 +3572,8 @@
       <c r="B63" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="C63" s="106"/>
-      <c r="D63" s="106"/>
+      <c r="C63" s="108"/>
+      <c r="D63" s="108"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
@@ -3619,6 +3619,28 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="F3:H5"/>
+    <mergeCell ref="C5:D7"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:C22"/>
+    <mergeCell ref="F21:H23"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:D25"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
     <mergeCell ref="C62:C63"/>
     <mergeCell ref="D62:D63"/>
     <mergeCell ref="A45:A46"/>
@@ -3631,28 +3653,6 @@
     <mergeCell ref="F48:F49"/>
     <mergeCell ref="G48:G49"/>
     <mergeCell ref="H48:H49"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:C22"/>
-    <mergeCell ref="F21:H23"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:D25"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="F3:H5"/>
-    <mergeCell ref="C5:D7"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="E5:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3681,46 +3681,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="114" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
-      <c r="J1" s="117"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="119"/>
     </row>
     <row r="2" spans="1:10" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="118" t="s">
+      <c r="A2" s="123" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
-      <c r="I2" s="118"/>
-      <c r="J2" s="119"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="124"/>
     </row>
     <row r="3" spans="1:10" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="118" t="s">
+      <c r="A3" s="123" t="s">
         <v>235</v>
       </c>
-      <c r="B3" s="118"/>
-      <c r="C3" s="118"/>
-      <c r="D3" s="118"/>
-      <c r="E3" s="118"/>
-      <c r="F3" s="118"/>
-      <c r="G3" s="118"/>
-      <c r="H3" s="118"/>
-      <c r="I3" s="118"/>
-      <c r="J3" s="119"/>
+      <c r="B3" s="123"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="123"/>
+      <c r="F3" s="123"/>
+      <c r="G3" s="123"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="123"/>
+      <c r="J3" s="124"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
@@ -4005,32 +4005,32 @@
       <c r="J13" s="63"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="118" t="s">
+      <c r="A14" s="123" t="s">
         <v>158</v>
       </c>
-      <c r="B14" s="118"/>
-      <c r="C14" s="118"/>
-      <c r="D14" s="118"/>
-      <c r="E14" s="118"/>
-      <c r="F14" s="118"/>
-      <c r="G14" s="118"/>
-      <c r="H14" s="118"/>
-      <c r="I14" s="118"/>
-      <c r="J14" s="119"/>
+      <c r="B14" s="123"/>
+      <c r="C14" s="123"/>
+      <c r="D14" s="123"/>
+      <c r="E14" s="123"/>
+      <c r="F14" s="123"/>
+      <c r="G14" s="123"/>
+      <c r="H14" s="123"/>
+      <c r="I14" s="123"/>
+      <c r="J14" s="124"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="118" t="s">
+      <c r="A15" s="123" t="s">
         <v>235</v>
       </c>
-      <c r="B15" s="118"/>
-      <c r="C15" s="118"/>
-      <c r="D15" s="118"/>
-      <c r="E15" s="118"/>
-      <c r="F15" s="118"/>
-      <c r="G15" s="118"/>
-      <c r="H15" s="118"/>
-      <c r="I15" s="118"/>
-      <c r="J15" s="119"/>
+      <c r="B15" s="123"/>
+      <c r="C15" s="123"/>
+      <c r="D15" s="123"/>
+      <c r="E15" s="123"/>
+      <c r="F15" s="123"/>
+      <c r="G15" s="123"/>
+      <c r="H15" s="123"/>
+      <c r="I15" s="123"/>
+      <c r="J15" s="124"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
@@ -4541,33 +4541,33 @@
       <c r="K32" s="11"/>
     </row>
     <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="118" t="s">
+      <c r="A33" s="123" t="s">
         <v>159</v>
       </c>
-      <c r="B33" s="118"/>
-      <c r="C33" s="118"/>
-      <c r="D33" s="118"/>
-      <c r="E33" s="118"/>
-      <c r="F33" s="118"/>
-      <c r="G33" s="118"/>
-      <c r="H33" s="118"/>
-      <c r="I33" s="118"/>
-      <c r="J33" s="119"/>
+      <c r="B33" s="123"/>
+      <c r="C33" s="123"/>
+      <c r="D33" s="123"/>
+      <c r="E33" s="123"/>
+      <c r="F33" s="123"/>
+      <c r="G33" s="123"/>
+      <c r="H33" s="123"/>
+      <c r="I33" s="123"/>
+      <c r="J33" s="124"/>
       <c r="K33" s="11"/>
     </row>
     <row r="34" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="118" t="s">
+      <c r="A34" s="123" t="s">
         <v>235</v>
       </c>
-      <c r="B34" s="118"/>
-      <c r="C34" s="118"/>
-      <c r="D34" s="118"/>
-      <c r="E34" s="118"/>
-      <c r="F34" s="118"/>
-      <c r="G34" s="118"/>
-      <c r="H34" s="118"/>
-      <c r="I34" s="118"/>
-      <c r="J34" s="119"/>
+      <c r="B34" s="123"/>
+      <c r="C34" s="123"/>
+      <c r="D34" s="123"/>
+      <c r="E34" s="123"/>
+      <c r="F34" s="123"/>
+      <c r="G34" s="123"/>
+      <c r="H34" s="123"/>
+      <c r="I34" s="123"/>
+      <c r="J34" s="124"/>
       <c r="K34" s="11"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -5086,17 +5086,17 @@
       <c r="K51" s="11"/>
     </row>
     <row r="52" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="118" t="s">
+      <c r="A52" s="123" t="s">
         <v>197</v>
       </c>
-      <c r="B52" s="118"/>
-      <c r="C52" s="118"/>
-      <c r="D52" s="118"/>
-      <c r="E52" s="118"/>
-      <c r="F52" s="118"/>
-      <c r="G52" s="118"/>
-      <c r="H52" s="118"/>
-      <c r="I52" s="119"/>
+      <c r="B52" s="123"/>
+      <c r="C52" s="123"/>
+      <c r="D52" s="123"/>
+      <c r="E52" s="123"/>
+      <c r="F52" s="123"/>
+      <c r="G52" s="123"/>
+      <c r="H52" s="123"/>
+      <c r="I52" s="124"/>
       <c r="J52" s="11"/>
       <c r="K52" s="11"/>
     </row>
@@ -5242,17 +5242,17 @@
       <c r="H58" s="11"/>
     </row>
     <row r="59" spans="1:11" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="118" t="s">
+      <c r="A59" s="123" t="s">
         <v>198</v>
       </c>
-      <c r="B59" s="118"/>
-      <c r="C59" s="118"/>
-      <c r="D59" s="118"/>
-      <c r="E59" s="118"/>
-      <c r="F59" s="118"/>
-      <c r="G59" s="118"/>
-      <c r="H59" s="118"/>
-      <c r="I59" s="119"/>
+      <c r="B59" s="123"/>
+      <c r="C59" s="123"/>
+      <c r="D59" s="123"/>
+      <c r="E59" s="123"/>
+      <c r="F59" s="123"/>
+      <c r="G59" s="123"/>
+      <c r="H59" s="123"/>
+      <c r="I59" s="124"/>
     </row>
     <row r="60" spans="1:11" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="26" t="s">
@@ -5406,17 +5406,17 @@
       <c r="H66" s="11"/>
     </row>
     <row r="67" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="118" t="s">
+      <c r="A67" s="123" t="s">
         <v>199</v>
       </c>
-      <c r="B67" s="118"/>
-      <c r="C67" s="118"/>
-      <c r="D67" s="118"/>
-      <c r="E67" s="118"/>
-      <c r="F67" s="118"/>
-      <c r="G67" s="118"/>
-      <c r="H67" s="118"/>
-      <c r="I67" s="119"/>
+      <c r="B67" s="123"/>
+      <c r="C67" s="123"/>
+      <c r="D67" s="123"/>
+      <c r="E67" s="123"/>
+      <c r="F67" s="123"/>
+      <c r="G67" s="123"/>
+      <c r="H67" s="123"/>
+      <c r="I67" s="124"/>
     </row>
     <row r="68" spans="1:9" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="26" t="s">
@@ -6175,17 +6175,17 @@
     </row>
     <row r="97" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="98" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="118" t="s">
+      <c r="A98" s="123" t="s">
         <v>200</v>
       </c>
-      <c r="B98" s="118"/>
-      <c r="C98" s="118"/>
-      <c r="D98" s="118"/>
-      <c r="E98" s="118"/>
-      <c r="F98" s="118"/>
-      <c r="G98" s="118"/>
-      <c r="H98" s="118"/>
-      <c r="I98" s="119"/>
+      <c r="B98" s="123"/>
+      <c r="C98" s="123"/>
+      <c r="D98" s="123"/>
+      <c r="E98" s="123"/>
+      <c r="F98" s="123"/>
+      <c r="G98" s="123"/>
+      <c r="H98" s="123"/>
+      <c r="I98" s="124"/>
     </row>
     <row r="99" spans="1:9" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="26" t="s">
@@ -6944,17 +6944,17 @@
     </row>
     <row r="128" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="129" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="118" t="s">
+      <c r="A129" s="123" t="s">
         <v>201</v>
       </c>
-      <c r="B129" s="118"/>
-      <c r="C129" s="118"/>
-      <c r="D129" s="118"/>
-      <c r="E129" s="118"/>
-      <c r="F129" s="118"/>
-      <c r="G129" s="118"/>
-      <c r="H129" s="118"/>
-      <c r="I129" s="119"/>
+      <c r="B129" s="123"/>
+      <c r="C129" s="123"/>
+      <c r="D129" s="123"/>
+      <c r="E129" s="123"/>
+      <c r="F129" s="123"/>
+      <c r="G129" s="123"/>
+      <c r="H129" s="123"/>
+      <c r="I129" s="124"/>
     </row>
     <row r="130" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="26" t="s">
@@ -7742,17 +7742,17 @@
     </row>
     <row r="160" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="161" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="118" t="s">
+      <c r="A161" s="123" t="s">
         <v>202</v>
       </c>
-      <c r="B161" s="118"/>
-      <c r="C161" s="118"/>
-      <c r="D161" s="118"/>
-      <c r="E161" s="118"/>
-      <c r="F161" s="118"/>
-      <c r="G161" s="118"/>
-      <c r="H161" s="118"/>
-      <c r="I161" s="119"/>
+      <c r="B161" s="123"/>
+      <c r="C161" s="123"/>
+      <c r="D161" s="123"/>
+      <c r="E161" s="123"/>
+      <c r="F161" s="123"/>
+      <c r="G161" s="123"/>
+      <c r="H161" s="123"/>
+      <c r="I161" s="124"/>
     </row>
     <row r="162" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="26" t="s">
@@ -8537,17 +8537,17 @@
     </row>
     <row r="192" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="193" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A193" s="118" t="s">
+      <c r="A193" s="123" t="s">
         <v>203</v>
       </c>
-      <c r="B193" s="118"/>
-      <c r="C193" s="118"/>
-      <c r="D193" s="118"/>
-      <c r="E193" s="118"/>
-      <c r="F193" s="118"/>
-      <c r="G193" s="118"/>
-      <c r="H193" s="118"/>
-      <c r="I193" s="119"/>
+      <c r="B193" s="123"/>
+      <c r="C193" s="123"/>
+      <c r="D193" s="123"/>
+      <c r="E193" s="123"/>
+      <c r="F193" s="123"/>
+      <c r="G193" s="123"/>
+      <c r="H193" s="123"/>
+      <c r="I193" s="124"/>
     </row>
     <row r="194" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="26" t="s">
@@ -9202,17 +9202,17 @@
     </row>
     <row r="219" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="220" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A220" s="118" t="s">
+      <c r="A220" s="123" t="s">
         <v>204</v>
       </c>
-      <c r="B220" s="118"/>
-      <c r="C220" s="118"/>
-      <c r="D220" s="118"/>
-      <c r="E220" s="118"/>
-      <c r="F220" s="118"/>
-      <c r="G220" s="118"/>
-      <c r="H220" s="118"/>
-      <c r="I220" s="119"/>
+      <c r="B220" s="123"/>
+      <c r="C220" s="123"/>
+      <c r="D220" s="123"/>
+      <c r="E220" s="123"/>
+      <c r="F220" s="123"/>
+      <c r="G220" s="123"/>
+      <c r="H220" s="123"/>
+      <c r="I220" s="124"/>
     </row>
     <row r="221" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A221" s="26" t="s">
@@ -9867,17 +9867,17 @@
     </row>
     <row r="246" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="247" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A247" s="118" t="s">
+      <c r="A247" s="123" t="s">
         <v>205</v>
       </c>
-      <c r="B247" s="118"/>
-      <c r="C247" s="118"/>
-      <c r="D247" s="118"/>
-      <c r="E247" s="118"/>
-      <c r="F247" s="118"/>
-      <c r="G247" s="118"/>
-      <c r="H247" s="118"/>
-      <c r="I247" s="119"/>
+      <c r="B247" s="123"/>
+      <c r="C247" s="123"/>
+      <c r="D247" s="123"/>
+      <c r="E247" s="123"/>
+      <c r="F247" s="123"/>
+      <c r="G247" s="123"/>
+      <c r="H247" s="123"/>
+      <c r="I247" s="124"/>
     </row>
     <row r="248" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A248" s="26" t="s">
@@ -10792,17 +10792,17 @@
     </row>
     <row r="283" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="284" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A284" s="118" t="s">
+      <c r="A284" s="123" t="s">
         <v>206</v>
       </c>
-      <c r="B284" s="118"/>
-      <c r="C284" s="118"/>
-      <c r="D284" s="118"/>
-      <c r="E284" s="118"/>
-      <c r="F284" s="118"/>
-      <c r="G284" s="118"/>
-      <c r="H284" s="118"/>
-      <c r="I284" s="119"/>
+      <c r="B284" s="123"/>
+      <c r="C284" s="123"/>
+      <c r="D284" s="123"/>
+      <c r="E284" s="123"/>
+      <c r="F284" s="123"/>
+      <c r="G284" s="123"/>
+      <c r="H284" s="123"/>
+      <c r="I284" s="124"/>
     </row>
     <row r="285" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A285" s="26" t="s">
@@ -11717,11 +11717,11 @@
     </row>
     <row r="320" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="321" spans="1:3" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A321" s="118" t="s">
+      <c r="A321" s="123" t="s">
         <v>161</v>
       </c>
-      <c r="B321" s="118"/>
-      <c r="C321" s="119"/>
+      <c r="B321" s="123"/>
+      <c r="C321" s="124"/>
     </row>
     <row r="322" spans="1:3" ht="81.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A322" s="26" t="s">
@@ -12090,7 +12090,7 @@
       <c r="A355" s="85">
         <v>2038</v>
       </c>
-      <c r="B355" s="129">
+      <c r="B355" s="102">
         <v>62</v>
       </c>
       <c r="C355" s="79">
@@ -12110,17 +12110,17 @@
     </row>
     <row r="357" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="358" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A358" s="118" t="s">
+      <c r="A358" s="123" t="s">
         <v>207</v>
       </c>
-      <c r="B358" s="118"/>
-      <c r="C358" s="118"/>
-      <c r="D358" s="118"/>
-      <c r="E358" s="118"/>
-      <c r="F358" s="118"/>
-      <c r="G358" s="118"/>
-      <c r="H358" s="118"/>
-      <c r="I358" s="119"/>
+      <c r="B358" s="123"/>
+      <c r="C358" s="123"/>
+      <c r="D358" s="123"/>
+      <c r="E358" s="123"/>
+      <c r="F358" s="123"/>
+      <c r="G358" s="123"/>
+      <c r="H358" s="123"/>
+      <c r="I358" s="124"/>
     </row>
     <row r="359" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A359" s="26" t="s">
@@ -12827,17 +12827,17 @@
     </row>
     <row r="386" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="387" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A387" s="118" t="s">
+      <c r="A387" s="123" t="s">
         <v>208</v>
       </c>
-      <c r="B387" s="118"/>
-      <c r="C387" s="118"/>
-      <c r="D387" s="118"/>
-      <c r="E387" s="118"/>
-      <c r="F387" s="118"/>
-      <c r="G387" s="118"/>
-      <c r="H387" s="118"/>
-      <c r="I387" s="119"/>
+      <c r="B387" s="123"/>
+      <c r="C387" s="123"/>
+      <c r="D387" s="123"/>
+      <c r="E387" s="123"/>
+      <c r="F387" s="123"/>
+      <c r="G387" s="123"/>
+      <c r="H387" s="123"/>
+      <c r="I387" s="124"/>
     </row>
     <row r="388" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A388" s="26" t="s">
@@ -13544,11 +13544,11 @@
     </row>
     <row r="415" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="416" spans="1:8" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A416" s="118" t="s">
+      <c r="A416" s="123" t="s">
         <v>163</v>
       </c>
-      <c r="B416" s="118"/>
-      <c r="C416" s="119"/>
+      <c r="B416" s="123"/>
+      <c r="C416" s="124"/>
     </row>
     <row r="417" spans="1:3" ht="81.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A417" s="26" t="s">
@@ -13849,10 +13849,10 @@
     </row>
     <row r="444" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="445" spans="1:3" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A445" s="118" t="s">
+      <c r="A445" s="123" t="s">
         <v>209</v>
       </c>
-      <c r="B445" s="119"/>
+      <c r="B445" s="124"/>
     </row>
     <row r="446" spans="1:3" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A446" s="26" t="s">
@@ -14080,10 +14080,10 @@
     </row>
     <row r="474" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="475" spans="1:2" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A475" s="118" t="s">
+      <c r="A475" s="123" t="s">
         <v>210</v>
       </c>
-      <c r="B475" s="119"/>
+      <c r="B475" s="124"/>
     </row>
     <row r="476" spans="1:2" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A476" s="26" t="s">
@@ -14311,10 +14311,10 @@
     </row>
     <row r="504" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="505" spans="1:2" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A505" s="118" t="s">
+      <c r="A505" s="123" t="s">
         <v>211</v>
       </c>
-      <c r="B505" s="119"/>
+      <c r="B505" s="124"/>
     </row>
     <row r="506" spans="1:2" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A506" s="26" t="s">
@@ -14464,7 +14464,7 @@
       <c r="A524" s="60">
         <v>2021</v>
       </c>
-      <c r="B524" s="130" t="s">
+      <c r="B524" s="103" t="s">
         <v>5</v>
       </c>
     </row>
@@ -14590,10 +14590,10 @@
     </row>
     <row r="540" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="541" spans="1:2" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A541" s="118" t="s">
+      <c r="A541" s="123" t="s">
         <v>212</v>
       </c>
-      <c r="B541" s="119"/>
+      <c r="B541" s="124"/>
     </row>
     <row r="542" spans="1:2" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A542" s="26" t="s">
@@ -14743,7 +14743,7 @@
       <c r="A560" s="60">
         <v>2021</v>
       </c>
-      <c r="B560" s="130" t="s">
+      <c r="B560" s="103" t="s">
         <v>5</v>
       </c>
     </row>
@@ -14869,72 +14869,72 @@
     </row>
     <row r="576" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="577" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A577" s="118" t="s">
+      <c r="A577" s="123" t="s">
         <v>213</v>
       </c>
-      <c r="B577" s="118"/>
-      <c r="C577" s="118"/>
-      <c r="D577" s="118"/>
-      <c r="E577" s="118"/>
-      <c r="F577" s="118"/>
-      <c r="G577" s="118"/>
-      <c r="H577" s="118"/>
+      <c r="B577" s="123"/>
+      <c r="C577" s="123"/>
+      <c r="D577" s="123"/>
+      <c r="E577" s="123"/>
+      <c r="F577" s="123"/>
+      <c r="G577" s="123"/>
+      <c r="H577" s="123"/>
     </row>
     <row r="578" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A578" s="104" t="s">
+      <c r="A578" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="B578" s="104" t="s">
+      <c r="B578" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="C578" s="104" t="s">
+      <c r="C578" s="107" t="s">
         <v>191</v>
       </c>
-      <c r="D578" s="104" t="s">
+      <c r="D578" s="107" t="s">
         <v>192</v>
       </c>
-      <c r="E578" s="104" t="s">
+      <c r="E578" s="107" t="s">
         <v>193</v>
       </c>
-      <c r="F578" s="104" t="s">
+      <c r="F578" s="107" t="s">
         <v>194</v>
       </c>
-      <c r="G578" s="104" t="s">
+      <c r="G578" s="107" t="s">
         <v>195</v>
       </c>
-      <c r="H578" s="104" t="s">
+      <c r="H578" s="107" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="579" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A579" s="105"/>
-      <c r="B579" s="105"/>
-      <c r="C579" s="105"/>
-      <c r="D579" s="105"/>
-      <c r="E579" s="105"/>
-      <c r="F579" s="105"/>
-      <c r="G579" s="105"/>
-      <c r="H579" s="105"/>
+      <c r="A579" s="122"/>
+      <c r="B579" s="122"/>
+      <c r="C579" s="122"/>
+      <c r="D579" s="122"/>
+      <c r="E579" s="122"/>
+      <c r="F579" s="122"/>
+      <c r="G579" s="122"/>
+      <c r="H579" s="122"/>
     </row>
     <row r="580" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A580" s="105"/>
-      <c r="B580" s="105"/>
-      <c r="C580" s="105"/>
-      <c r="D580" s="105"/>
-      <c r="E580" s="105"/>
-      <c r="F580" s="105"/>
-      <c r="G580" s="105"/>
-      <c r="H580" s="105"/>
+      <c r="A580" s="122"/>
+      <c r="B580" s="122"/>
+      <c r="C580" s="122"/>
+      <c r="D580" s="122"/>
+      <c r="E580" s="122"/>
+      <c r="F580" s="122"/>
+      <c r="G580" s="122"/>
+      <c r="H580" s="122"/>
     </row>
     <row r="581" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A581" s="106"/>
-      <c r="B581" s="106"/>
-      <c r="C581" s="106"/>
-      <c r="D581" s="106"/>
-      <c r="E581" s="106"/>
-      <c r="F581" s="106"/>
-      <c r="G581" s="106"/>
-      <c r="H581" s="106"/>
+      <c r="A581" s="108"/>
+      <c r="B581" s="108"/>
+      <c r="C581" s="108"/>
+      <c r="D581" s="108"/>
+      <c r="E581" s="108"/>
+      <c r="F581" s="108"/>
+      <c r="G581" s="108"/>
+      <c r="H581" s="108"/>
     </row>
     <row r="582" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A582" s="8">
@@ -15562,17 +15562,17 @@
     </row>
     <row r="606" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="607" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A607" s="118" t="s">
+      <c r="A607" s="123" t="s">
         <v>214</v>
       </c>
-      <c r="B607" s="118"/>
-      <c r="C607" s="118"/>
-      <c r="D607" s="118"/>
-      <c r="E607" s="118"/>
-      <c r="F607" s="118"/>
-      <c r="G607" s="118"/>
-      <c r="H607" s="118"/>
-      <c r="I607" s="119"/>
+      <c r="B607" s="123"/>
+      <c r="C607" s="123"/>
+      <c r="D607" s="123"/>
+      <c r="E607" s="123"/>
+      <c r="F607" s="123"/>
+      <c r="G607" s="123"/>
+      <c r="H607" s="123"/>
+      <c r="I607" s="124"/>
     </row>
     <row r="608" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A608" s="26" t="s">
@@ -16227,72 +16227,72 @@
     </row>
     <row r="633" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="634" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A634" s="118" t="s">
+      <c r="A634" s="123" t="s">
         <v>215</v>
       </c>
-      <c r="B634" s="118"/>
-      <c r="C634" s="118"/>
-      <c r="D634" s="118"/>
-      <c r="E634" s="118"/>
-      <c r="F634" s="118"/>
-      <c r="G634" s="118"/>
-      <c r="H634" s="118"/>
+      <c r="B634" s="123"/>
+      <c r="C634" s="123"/>
+      <c r="D634" s="123"/>
+      <c r="E634" s="123"/>
+      <c r="F634" s="123"/>
+      <c r="G634" s="123"/>
+      <c r="H634" s="123"/>
     </row>
     <row r="635" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A635" s="104" t="s">
+      <c r="A635" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="B635" s="104" t="s">
+      <c r="B635" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="C635" s="104" t="s">
+      <c r="C635" s="107" t="s">
         <v>191</v>
       </c>
-      <c r="D635" s="104" t="s">
+      <c r="D635" s="107" t="s">
         <v>192</v>
       </c>
-      <c r="E635" s="104" t="s">
+      <c r="E635" s="107" t="s">
         <v>193</v>
       </c>
-      <c r="F635" s="104" t="s">
+      <c r="F635" s="107" t="s">
         <v>194</v>
       </c>
-      <c r="G635" s="104" t="s">
+      <c r="G635" s="107" t="s">
         <v>195</v>
       </c>
-      <c r="H635" s="104" t="s">
+      <c r="H635" s="107" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="636" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A636" s="105"/>
-      <c r="B636" s="105"/>
-      <c r="C636" s="105"/>
-      <c r="D636" s="105"/>
-      <c r="E636" s="105"/>
-      <c r="F636" s="105"/>
-      <c r="G636" s="105"/>
-      <c r="H636" s="105"/>
+      <c r="A636" s="122"/>
+      <c r="B636" s="122"/>
+      <c r="C636" s="122"/>
+      <c r="D636" s="122"/>
+      <c r="E636" s="122"/>
+      <c r="F636" s="122"/>
+      <c r="G636" s="122"/>
+      <c r="H636" s="122"/>
     </row>
     <row r="637" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A637" s="105"/>
-      <c r="B637" s="105"/>
-      <c r="C637" s="105"/>
-      <c r="D637" s="105"/>
-      <c r="E637" s="105"/>
-      <c r="F637" s="105"/>
-      <c r="G637" s="105"/>
-      <c r="H637" s="105"/>
+      <c r="A637" s="122"/>
+      <c r="B637" s="122"/>
+      <c r="C637" s="122"/>
+      <c r="D637" s="122"/>
+      <c r="E637" s="122"/>
+      <c r="F637" s="122"/>
+      <c r="G637" s="122"/>
+      <c r="H637" s="122"/>
     </row>
     <row r="638" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A638" s="106"/>
-      <c r="B638" s="106"/>
-      <c r="C638" s="106"/>
-      <c r="D638" s="106"/>
-      <c r="E638" s="106"/>
-      <c r="F638" s="106"/>
-      <c r="G638" s="106"/>
-      <c r="H638" s="106"/>
+      <c r="A638" s="108"/>
+      <c r="B638" s="108"/>
+      <c r="C638" s="108"/>
+      <c r="D638" s="108"/>
+      <c r="E638" s="108"/>
+      <c r="F638" s="108"/>
+      <c r="G638" s="108"/>
+      <c r="H638" s="108"/>
     </row>
     <row r="639" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A639" s="8">
@@ -16946,17 +16946,17 @@
     </row>
     <row r="664" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="665" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A665" s="118" t="s">
+      <c r="A665" s="123" t="s">
         <v>216</v>
       </c>
-      <c r="B665" s="118"/>
-      <c r="C665" s="118"/>
-      <c r="D665" s="118"/>
-      <c r="E665" s="118"/>
-      <c r="F665" s="118"/>
-      <c r="G665" s="118"/>
-      <c r="H665" s="118"/>
-      <c r="I665" s="119"/>
+      <c r="B665" s="123"/>
+      <c r="C665" s="123"/>
+      <c r="D665" s="123"/>
+      <c r="E665" s="123"/>
+      <c r="F665" s="123"/>
+      <c r="G665" s="123"/>
+      <c r="H665" s="123"/>
+      <c r="I665" s="124"/>
     </row>
     <row r="666" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A666" s="26" t="s">
@@ -17637,72 +17637,72 @@
     </row>
     <row r="692" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="693" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A693" s="118" t="s">
+      <c r="A693" s="123" t="s">
         <v>217</v>
       </c>
-      <c r="B693" s="118"/>
-      <c r="C693" s="118"/>
-      <c r="D693" s="118"/>
-      <c r="E693" s="118"/>
-      <c r="F693" s="118"/>
-      <c r="G693" s="118"/>
-      <c r="H693" s="118"/>
+      <c r="B693" s="123"/>
+      <c r="C693" s="123"/>
+      <c r="D693" s="123"/>
+      <c r="E693" s="123"/>
+      <c r="F693" s="123"/>
+      <c r="G693" s="123"/>
+      <c r="H693" s="123"/>
     </row>
     <row r="694" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A694" s="104" t="s">
+      <c r="A694" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="B694" s="104" t="s">
+      <c r="B694" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="C694" s="104" t="s">
+      <c r="C694" s="107" t="s">
         <v>191</v>
       </c>
-      <c r="D694" s="104" t="s">
+      <c r="D694" s="107" t="s">
         <v>192</v>
       </c>
-      <c r="E694" s="104" t="s">
+      <c r="E694" s="107" t="s">
         <v>193</v>
       </c>
-      <c r="F694" s="104" t="s">
+      <c r="F694" s="107" t="s">
         <v>194</v>
       </c>
-      <c r="G694" s="104" t="s">
+      <c r="G694" s="107" t="s">
         <v>195</v>
       </c>
-      <c r="H694" s="104" t="s">
+      <c r="H694" s="107" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="695" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A695" s="105"/>
-      <c r="B695" s="105"/>
-      <c r="C695" s="105"/>
-      <c r="D695" s="105"/>
-      <c r="E695" s="105"/>
-      <c r="F695" s="105"/>
-      <c r="G695" s="105"/>
-      <c r="H695" s="105"/>
+      <c r="A695" s="122"/>
+      <c r="B695" s="122"/>
+      <c r="C695" s="122"/>
+      <c r="D695" s="122"/>
+      <c r="E695" s="122"/>
+      <c r="F695" s="122"/>
+      <c r="G695" s="122"/>
+      <c r="H695" s="122"/>
     </row>
     <row r="696" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A696" s="105"/>
-      <c r="B696" s="105"/>
-      <c r="C696" s="105"/>
-      <c r="D696" s="105"/>
-      <c r="E696" s="105"/>
-      <c r="F696" s="105"/>
-      <c r="G696" s="105"/>
-      <c r="H696" s="105"/>
+      <c r="A696" s="122"/>
+      <c r="B696" s="122"/>
+      <c r="C696" s="122"/>
+      <c r="D696" s="122"/>
+      <c r="E696" s="122"/>
+      <c r="F696" s="122"/>
+      <c r="G696" s="122"/>
+      <c r="H696" s="122"/>
     </row>
     <row r="697" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A697" s="106"/>
-      <c r="B697" s="106"/>
-      <c r="C697" s="106"/>
-      <c r="D697" s="106"/>
-      <c r="E697" s="106"/>
-      <c r="F697" s="106"/>
-      <c r="G697" s="106"/>
-      <c r="H697" s="106"/>
+      <c r="A697" s="108"/>
+      <c r="B697" s="108"/>
+      <c r="C697" s="108"/>
+      <c r="D697" s="108"/>
+      <c r="E697" s="108"/>
+      <c r="F697" s="108"/>
+      <c r="G697" s="108"/>
+      <c r="H697" s="108"/>
     </row>
     <row r="698" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A698" s="8">
@@ -17810,17 +17810,17 @@
     </row>
     <row r="702" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="703" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A703" s="118" t="s">
+      <c r="A703" s="123" t="s">
         <v>218</v>
       </c>
-      <c r="B703" s="118"/>
-      <c r="C703" s="118"/>
-      <c r="D703" s="118"/>
-      <c r="E703" s="118"/>
-      <c r="F703" s="118"/>
-      <c r="G703" s="118"/>
-      <c r="H703" s="118"/>
-      <c r="I703" s="119"/>
+      <c r="B703" s="123"/>
+      <c r="C703" s="123"/>
+      <c r="D703" s="123"/>
+      <c r="E703" s="123"/>
+      <c r="F703" s="123"/>
+      <c r="G703" s="123"/>
+      <c r="H703" s="123"/>
+      <c r="I703" s="124"/>
     </row>
     <row r="704" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A704" s="26" t="s">
@@ -17955,72 +17955,72 @@
     </row>
     <row r="709" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="710" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A710" s="118" t="s">
+      <c r="A710" s="123" t="s">
         <v>219</v>
       </c>
-      <c r="B710" s="118"/>
-      <c r="C710" s="118"/>
-      <c r="D710" s="118"/>
-      <c r="E710" s="118"/>
-      <c r="F710" s="118"/>
-      <c r="G710" s="118"/>
-      <c r="H710" s="118"/>
+      <c r="B710" s="123"/>
+      <c r="C710" s="123"/>
+      <c r="D710" s="123"/>
+      <c r="E710" s="123"/>
+      <c r="F710" s="123"/>
+      <c r="G710" s="123"/>
+      <c r="H710" s="123"/>
     </row>
     <row r="711" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A711" s="104" t="s">
+      <c r="A711" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="B711" s="104" t="s">
+      <c r="B711" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="C711" s="104" t="s">
+      <c r="C711" s="107" t="s">
         <v>191</v>
       </c>
-      <c r="D711" s="104" t="s">
+      <c r="D711" s="107" t="s">
         <v>192</v>
       </c>
-      <c r="E711" s="104" t="s">
+      <c r="E711" s="107" t="s">
         <v>193</v>
       </c>
-      <c r="F711" s="104" t="s">
+      <c r="F711" s="107" t="s">
         <v>194</v>
       </c>
-      <c r="G711" s="104" t="s">
+      <c r="G711" s="107" t="s">
         <v>195</v>
       </c>
-      <c r="H711" s="104" t="s">
+      <c r="H711" s="107" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="712" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A712" s="105"/>
-      <c r="B712" s="105"/>
-      <c r="C712" s="105"/>
-      <c r="D712" s="105"/>
-      <c r="E712" s="105"/>
-      <c r="F712" s="105"/>
-      <c r="G712" s="105"/>
-      <c r="H712" s="105"/>
+      <c r="A712" s="122"/>
+      <c r="B712" s="122"/>
+      <c r="C712" s="122"/>
+      <c r="D712" s="122"/>
+      <c r="E712" s="122"/>
+      <c r="F712" s="122"/>
+      <c r="G712" s="122"/>
+      <c r="H712" s="122"/>
     </row>
     <row r="713" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A713" s="105"/>
-      <c r="B713" s="105"/>
-      <c r="C713" s="105"/>
-      <c r="D713" s="105"/>
-      <c r="E713" s="105"/>
-      <c r="F713" s="105"/>
-      <c r="G713" s="105"/>
-      <c r="H713" s="105"/>
+      <c r="A713" s="122"/>
+      <c r="B713" s="122"/>
+      <c r="C713" s="122"/>
+      <c r="D713" s="122"/>
+      <c r="E713" s="122"/>
+      <c r="F713" s="122"/>
+      <c r="G713" s="122"/>
+      <c r="H713" s="122"/>
     </row>
     <row r="714" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A714" s="106"/>
-      <c r="B714" s="106"/>
-      <c r="C714" s="106"/>
-      <c r="D714" s="106"/>
-      <c r="E714" s="106"/>
-      <c r="F714" s="106"/>
-      <c r="G714" s="106"/>
-      <c r="H714" s="106"/>
+      <c r="A714" s="108"/>
+      <c r="B714" s="108"/>
+      <c r="C714" s="108"/>
+      <c r="D714" s="108"/>
+      <c r="E714" s="108"/>
+      <c r="F714" s="108"/>
+      <c r="G714" s="108"/>
+      <c r="H714" s="108"/>
     </row>
     <row r="715" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A715" s="8">
@@ -18518,17 +18518,17 @@
     </row>
     <row r="734" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="735" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A735" s="118" t="s">
+      <c r="A735" s="123" t="s">
         <v>220</v>
       </c>
-      <c r="B735" s="118"/>
-      <c r="C735" s="118"/>
-      <c r="D735" s="118"/>
-      <c r="E735" s="118"/>
-      <c r="F735" s="118"/>
-      <c r="G735" s="118"/>
-      <c r="H735" s="118"/>
-      <c r="I735" s="119"/>
+      <c r="B735" s="123"/>
+      <c r="C735" s="123"/>
+      <c r="D735" s="123"/>
+      <c r="E735" s="123"/>
+      <c r="F735" s="123"/>
+      <c r="G735" s="123"/>
+      <c r="H735" s="123"/>
+      <c r="I735" s="124"/>
     </row>
     <row r="736" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A736" s="26" t="s">
@@ -19053,72 +19053,72 @@
     </row>
     <row r="756" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="757" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A757" s="118" t="s">
+      <c r="A757" s="123" t="s">
         <v>221</v>
       </c>
-      <c r="B757" s="118"/>
-      <c r="C757" s="118"/>
-      <c r="D757" s="118"/>
-      <c r="E757" s="118"/>
-      <c r="F757" s="118"/>
-      <c r="G757" s="118"/>
-      <c r="H757" s="118"/>
+      <c r="B757" s="123"/>
+      <c r="C757" s="123"/>
+      <c r="D757" s="123"/>
+      <c r="E757" s="123"/>
+      <c r="F757" s="123"/>
+      <c r="G757" s="123"/>
+      <c r="H757" s="123"/>
     </row>
     <row r="758" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A758" s="104" t="s">
+      <c r="A758" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="B758" s="104" t="s">
+      <c r="B758" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="C758" s="104" t="s">
+      <c r="C758" s="107" t="s">
         <v>191</v>
       </c>
-      <c r="D758" s="104" t="s">
+      <c r="D758" s="107" t="s">
         <v>192</v>
       </c>
-      <c r="E758" s="104" t="s">
+      <c r="E758" s="107" t="s">
         <v>193</v>
       </c>
-      <c r="F758" s="104" t="s">
+      <c r="F758" s="107" t="s">
         <v>194</v>
       </c>
-      <c r="G758" s="104" t="s">
+      <c r="G758" s="107" t="s">
         <v>195</v>
       </c>
-      <c r="H758" s="104" t="s">
+      <c r="H758" s="107" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="759" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A759" s="105"/>
-      <c r="B759" s="105"/>
-      <c r="C759" s="105"/>
-      <c r="D759" s="105"/>
-      <c r="E759" s="105"/>
-      <c r="F759" s="105"/>
-      <c r="G759" s="105"/>
-      <c r="H759" s="105"/>
+      <c r="A759" s="122"/>
+      <c r="B759" s="122"/>
+      <c r="C759" s="122"/>
+      <c r="D759" s="122"/>
+      <c r="E759" s="122"/>
+      <c r="F759" s="122"/>
+      <c r="G759" s="122"/>
+      <c r="H759" s="122"/>
     </row>
     <row r="760" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A760" s="105"/>
-      <c r="B760" s="105"/>
-      <c r="C760" s="105"/>
-      <c r="D760" s="105"/>
-      <c r="E760" s="105"/>
-      <c r="F760" s="105"/>
-      <c r="G760" s="105"/>
-      <c r="H760" s="105"/>
+      <c r="A760" s="122"/>
+      <c r="B760" s="122"/>
+      <c r="C760" s="122"/>
+      <c r="D760" s="122"/>
+      <c r="E760" s="122"/>
+      <c r="F760" s="122"/>
+      <c r="G760" s="122"/>
+      <c r="H760" s="122"/>
     </row>
     <row r="761" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A761" s="106"/>
-      <c r="B761" s="106"/>
-      <c r="C761" s="106"/>
-      <c r="D761" s="106"/>
-      <c r="E761" s="106"/>
-      <c r="F761" s="106"/>
-      <c r="G761" s="106"/>
-      <c r="H761" s="106"/>
+      <c r="A761" s="108"/>
+      <c r="B761" s="108"/>
+      <c r="C761" s="108"/>
+      <c r="D761" s="108"/>
+      <c r="E761" s="108"/>
+      <c r="F761" s="108"/>
+      <c r="G761" s="108"/>
+      <c r="H761" s="108"/>
     </row>
     <row r="762" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A762" s="36">
@@ -20006,17 +20006,17 @@
     </row>
     <row r="796" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="797" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A797" s="118" t="s">
+      <c r="A797" s="123" t="s">
         <v>222</v>
       </c>
-      <c r="B797" s="118"/>
-      <c r="C797" s="118"/>
-      <c r="D797" s="118"/>
-      <c r="E797" s="118"/>
-      <c r="F797" s="118"/>
-      <c r="G797" s="118"/>
-      <c r="H797" s="118"/>
-      <c r="I797" s="119"/>
+      <c r="B797" s="123"/>
+      <c r="C797" s="123"/>
+      <c r="D797" s="123"/>
+      <c r="E797" s="123"/>
+      <c r="F797" s="123"/>
+      <c r="G797" s="123"/>
+      <c r="H797" s="123"/>
+      <c r="I797" s="124"/>
     </row>
     <row r="798" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A798" s="26" t="s">
@@ -20931,11 +20931,11 @@
     </row>
     <row r="833" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="834" spans="1:3" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A834" s="118" t="s">
+      <c r="A834" s="123" t="s">
         <v>164</v>
       </c>
-      <c r="B834" s="118"/>
-      <c r="C834" s="119"/>
+      <c r="B834" s="123"/>
+      <c r="C834" s="124"/>
     </row>
     <row r="835" spans="1:3" ht="81.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A835" s="26" t="s">
@@ -21304,7 +21304,7 @@
       <c r="A868" s="85">
         <v>2038</v>
       </c>
-      <c r="B868" s="129">
+      <c r="B868" s="102">
         <v>62</v>
       </c>
       <c r="C868" s="79">
@@ -21324,72 +21324,72 @@
     </row>
     <row r="870" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="871" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A871" s="118" t="s">
+      <c r="A871" s="123" t="s">
         <v>223</v>
       </c>
-      <c r="B871" s="118"/>
-      <c r="C871" s="118"/>
-      <c r="D871" s="118"/>
-      <c r="E871" s="118"/>
-      <c r="F871" s="118"/>
-      <c r="G871" s="118"/>
-      <c r="H871" s="118"/>
+      <c r="B871" s="123"/>
+      <c r="C871" s="123"/>
+      <c r="D871" s="123"/>
+      <c r="E871" s="123"/>
+      <c r="F871" s="123"/>
+      <c r="G871" s="123"/>
+      <c r="H871" s="123"/>
     </row>
     <row r="872" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A872" s="104" t="s">
+      <c r="A872" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="B872" s="104" t="s">
+      <c r="B872" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="C872" s="104" t="s">
+      <c r="C872" s="107" t="s">
         <v>191</v>
       </c>
-      <c r="D872" s="104" t="s">
+      <c r="D872" s="107" t="s">
         <v>192</v>
       </c>
-      <c r="E872" s="104" t="s">
+      <c r="E872" s="107" t="s">
         <v>193</v>
       </c>
-      <c r="F872" s="104" t="s">
+      <c r="F872" s="107" t="s">
         <v>194</v>
       </c>
-      <c r="G872" s="104" t="s">
+      <c r="G872" s="107" t="s">
         <v>195</v>
       </c>
-      <c r="H872" s="104" t="s">
+      <c r="H872" s="107" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="873" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A873" s="105"/>
-      <c r="B873" s="105"/>
-      <c r="C873" s="105"/>
-      <c r="D873" s="105"/>
-      <c r="E873" s="105"/>
-      <c r="F873" s="105"/>
-      <c r="G873" s="105"/>
-      <c r="H873" s="105"/>
+      <c r="A873" s="122"/>
+      <c r="B873" s="122"/>
+      <c r="C873" s="122"/>
+      <c r="D873" s="122"/>
+      <c r="E873" s="122"/>
+      <c r="F873" s="122"/>
+      <c r="G873" s="122"/>
+      <c r="H873" s="122"/>
     </row>
     <row r="874" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A874" s="105"/>
-      <c r="B874" s="105"/>
-      <c r="C874" s="105"/>
-      <c r="D874" s="105"/>
-      <c r="E874" s="105"/>
-      <c r="F874" s="105"/>
-      <c r="G874" s="105"/>
-      <c r="H874" s="105"/>
+      <c r="A874" s="122"/>
+      <c r="B874" s="122"/>
+      <c r="C874" s="122"/>
+      <c r="D874" s="122"/>
+      <c r="E874" s="122"/>
+      <c r="F874" s="122"/>
+      <c r="G874" s="122"/>
+      <c r="H874" s="122"/>
     </row>
     <row r="875" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A875" s="106"/>
-      <c r="B875" s="106"/>
-      <c r="C875" s="106"/>
-      <c r="D875" s="106"/>
-      <c r="E875" s="106"/>
-      <c r="F875" s="106"/>
-      <c r="G875" s="106"/>
-      <c r="H875" s="106"/>
+      <c r="A875" s="108"/>
+      <c r="B875" s="108"/>
+      <c r="C875" s="108"/>
+      <c r="D875" s="108"/>
+      <c r="E875" s="108"/>
+      <c r="F875" s="108"/>
+      <c r="G875" s="108"/>
+      <c r="H875" s="108"/>
     </row>
     <row r="876" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A876" s="36">
@@ -22078,17 +22078,17 @@
       <c r="H902" s="8"/>
     </row>
     <row r="903" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A903" s="118" t="s">
+      <c r="A903" s="123" t="s">
         <v>224</v>
       </c>
-      <c r="B903" s="118"/>
-      <c r="C903" s="118"/>
-      <c r="D903" s="118"/>
-      <c r="E903" s="118"/>
-      <c r="F903" s="118"/>
-      <c r="G903" s="118"/>
-      <c r="H903" s="118"/>
-      <c r="I903" s="119"/>
+      <c r="B903" s="123"/>
+      <c r="C903" s="123"/>
+      <c r="D903" s="123"/>
+      <c r="E903" s="123"/>
+      <c r="F903" s="123"/>
+      <c r="G903" s="123"/>
+      <c r="H903" s="123"/>
+      <c r="I903" s="124"/>
     </row>
     <row r="904" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A904" s="26" t="s">
@@ -22804,11 +22804,11 @@
       <c r="H931" s="8"/>
     </row>
     <row r="932" spans="1:8" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A932" s="118" t="s">
+      <c r="A932" s="123" t="s">
         <v>165</v>
       </c>
-      <c r="B932" s="118"/>
-      <c r="C932" s="119"/>
+      <c r="B932" s="123"/>
+      <c r="C932" s="124"/>
     </row>
     <row r="933" spans="1:8" ht="81.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A933" s="26" t="s">
@@ -23109,67 +23109,16 @@
     </row>
   </sheetData>
   <mergeCells count="87">
-    <mergeCell ref="A358:I358"/>
-    <mergeCell ref="A387:I387"/>
-    <mergeCell ref="A161:I161"/>
-    <mergeCell ref="A193:I193"/>
-    <mergeCell ref="A220:I220"/>
-    <mergeCell ref="A247:I247"/>
-    <mergeCell ref="A284:I284"/>
-    <mergeCell ref="A735:I735"/>
-    <mergeCell ref="A757:H757"/>
-    <mergeCell ref="A758:A761"/>
-    <mergeCell ref="B758:B761"/>
-    <mergeCell ref="C758:C761"/>
-    <mergeCell ref="D758:D761"/>
-    <mergeCell ref="E758:E761"/>
-    <mergeCell ref="F758:F761"/>
-    <mergeCell ref="G758:G761"/>
-    <mergeCell ref="H758:H761"/>
-    <mergeCell ref="A703:I703"/>
-    <mergeCell ref="A710:H710"/>
-    <mergeCell ref="A711:A714"/>
-    <mergeCell ref="B711:B714"/>
-    <mergeCell ref="C711:C714"/>
-    <mergeCell ref="D711:D714"/>
-    <mergeCell ref="E711:E714"/>
-    <mergeCell ref="F711:F714"/>
-    <mergeCell ref="G711:G714"/>
-    <mergeCell ref="H711:H714"/>
-    <mergeCell ref="A665:I665"/>
-    <mergeCell ref="A693:H693"/>
-    <mergeCell ref="A694:A697"/>
-    <mergeCell ref="B694:B697"/>
-    <mergeCell ref="C694:C697"/>
-    <mergeCell ref="D694:D697"/>
-    <mergeCell ref="E694:E697"/>
-    <mergeCell ref="F694:F697"/>
-    <mergeCell ref="G694:G697"/>
-    <mergeCell ref="H694:H697"/>
-    <mergeCell ref="G635:G638"/>
-    <mergeCell ref="H635:H638"/>
-    <mergeCell ref="C578:C581"/>
-    <mergeCell ref="D578:D581"/>
-    <mergeCell ref="E578:E581"/>
-    <mergeCell ref="F578:F581"/>
-    <mergeCell ref="G578:G581"/>
-    <mergeCell ref="B635:B638"/>
-    <mergeCell ref="C635:C638"/>
-    <mergeCell ref="D635:D638"/>
-    <mergeCell ref="E635:E638"/>
-    <mergeCell ref="F635:F638"/>
-    <mergeCell ref="A59:I59"/>
-    <mergeCell ref="A98:I98"/>
-    <mergeCell ref="A67:I67"/>
-    <mergeCell ref="A129:I129"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A52:I52"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A14:J14"/>
-    <mergeCell ref="A15:J15"/>
-    <mergeCell ref="A33:J33"/>
-    <mergeCell ref="A34:J34"/>
+    <mergeCell ref="F872:F875"/>
+    <mergeCell ref="G872:G875"/>
+    <mergeCell ref="H872:H875"/>
+    <mergeCell ref="A903:I903"/>
+    <mergeCell ref="A932:C932"/>
+    <mergeCell ref="A872:A875"/>
+    <mergeCell ref="B872:B875"/>
+    <mergeCell ref="C872:C875"/>
+    <mergeCell ref="D872:D875"/>
+    <mergeCell ref="E872:E875"/>
     <mergeCell ref="A797:I797"/>
     <mergeCell ref="A834:C834"/>
     <mergeCell ref="A871:H871"/>
@@ -23186,16 +23135,67 @@
     <mergeCell ref="A607:I607"/>
     <mergeCell ref="A634:H634"/>
     <mergeCell ref="A635:A638"/>
-    <mergeCell ref="F872:F875"/>
-    <mergeCell ref="G872:G875"/>
-    <mergeCell ref="H872:H875"/>
-    <mergeCell ref="A903:I903"/>
-    <mergeCell ref="A932:C932"/>
-    <mergeCell ref="A872:A875"/>
-    <mergeCell ref="B872:B875"/>
-    <mergeCell ref="C872:C875"/>
-    <mergeCell ref="D872:D875"/>
-    <mergeCell ref="E872:E875"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A52:I52"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A14:J14"/>
+    <mergeCell ref="A15:J15"/>
+    <mergeCell ref="A33:J33"/>
+    <mergeCell ref="A34:J34"/>
+    <mergeCell ref="A59:I59"/>
+    <mergeCell ref="A98:I98"/>
+    <mergeCell ref="A67:I67"/>
+    <mergeCell ref="A129:I129"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="B635:B638"/>
+    <mergeCell ref="C635:C638"/>
+    <mergeCell ref="D635:D638"/>
+    <mergeCell ref="E635:E638"/>
+    <mergeCell ref="F635:F638"/>
+    <mergeCell ref="G635:G638"/>
+    <mergeCell ref="H635:H638"/>
+    <mergeCell ref="C578:C581"/>
+    <mergeCell ref="D578:D581"/>
+    <mergeCell ref="E578:E581"/>
+    <mergeCell ref="F578:F581"/>
+    <mergeCell ref="G578:G581"/>
+    <mergeCell ref="A665:I665"/>
+    <mergeCell ref="A693:H693"/>
+    <mergeCell ref="A694:A697"/>
+    <mergeCell ref="B694:B697"/>
+    <mergeCell ref="C694:C697"/>
+    <mergeCell ref="D694:D697"/>
+    <mergeCell ref="E694:E697"/>
+    <mergeCell ref="F694:F697"/>
+    <mergeCell ref="G694:G697"/>
+    <mergeCell ref="H694:H697"/>
+    <mergeCell ref="A703:I703"/>
+    <mergeCell ref="A710:H710"/>
+    <mergeCell ref="A711:A714"/>
+    <mergeCell ref="B711:B714"/>
+    <mergeCell ref="C711:C714"/>
+    <mergeCell ref="D711:D714"/>
+    <mergeCell ref="E711:E714"/>
+    <mergeCell ref="F711:F714"/>
+    <mergeCell ref="G711:G714"/>
+    <mergeCell ref="H711:H714"/>
+    <mergeCell ref="A735:I735"/>
+    <mergeCell ref="A757:H757"/>
+    <mergeCell ref="A758:A761"/>
+    <mergeCell ref="B758:B761"/>
+    <mergeCell ref="C758:C761"/>
+    <mergeCell ref="D758:D761"/>
+    <mergeCell ref="E758:E761"/>
+    <mergeCell ref="F758:F761"/>
+    <mergeCell ref="G758:G761"/>
+    <mergeCell ref="H758:H761"/>
+    <mergeCell ref="A358:I358"/>
+    <mergeCell ref="A387:I387"/>
+    <mergeCell ref="A161:I161"/>
+    <mergeCell ref="A193:I193"/>
+    <mergeCell ref="A220:I220"/>
+    <mergeCell ref="A247:I247"/>
+    <mergeCell ref="A284:I284"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23218,11 +23218,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="123" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="119"/>
+      <c r="B1" s="123"/>
+      <c r="C1" s="124"/>
     </row>
     <row r="2" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26"/>
@@ -23290,11 +23290,11 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="118" t="s">
+      <c r="A9" s="123" t="s">
         <v>167</v>
       </c>
-      <c r="B9" s="118"/>
-      <c r="C9" s="119"/>
+      <c r="B9" s="123"/>
+      <c r="C9" s="124"/>
     </row>
     <row r="10" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="26"/>
@@ -23384,13 +23384,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="125" t="s">
         <v>168</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="121"/>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="126"/>
     </row>
     <row r="2" spans="1:5" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
@@ -23463,8 +23463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J108"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="F103" sqref="F103"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23519,10 +23519,10 @@
       <c r="A5" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="131">
+      <c r="B5" s="104">
         <v>274958.40000000002</v>
       </c>
-      <c r="C5" s="131">
+      <c r="C5" s="104">
         <v>261760.9</v>
       </c>
     </row>
@@ -23561,10 +23561,10 @@
       <c r="A9" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="131">
+      <c r="B9" s="104">
         <v>224332.9</v>
       </c>
-      <c r="C9" s="131">
+      <c r="C9" s="104">
         <v>211290.9</v>
       </c>
     </row>
@@ -23627,10 +23627,10 @@
       <c r="A16" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="131">
+      <c r="B16" s="104">
         <v>276482.2</v>
       </c>
-      <c r="C16" s="131">
+      <c r="C16" s="104">
         <v>261760.9</v>
       </c>
     </row>
@@ -23669,10 +23669,10 @@
       <c r="A20" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="131">
+      <c r="B20" s="104">
         <v>224333.7</v>
       </c>
-      <c r="C20" s="131">
+      <c r="C20" s="104">
         <v>211290.9</v>
       </c>
     </row>
@@ -23707,14 +23707,14 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="122" t="s">
+      <c r="C25" s="127" t="s">
         <v>149</v>
       </c>
-      <c r="D25" s="119"/>
-      <c r="E25" s="122" t="s">
+      <c r="D25" s="124"/>
+      <c r="E25" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="119"/>
+      <c r="F25" s="124"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="26" t="s">
@@ -23878,17 +23878,17 @@
       <c r="A35" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="122" t="s">
+      <c r="B35" s="127" t="s">
         <v>69</v>
       </c>
-      <c r="C35" s="118"/>
-      <c r="D35" s="118"/>
-      <c r="E35" s="118"/>
-      <c r="F35" s="118"/>
-      <c r="G35" s="118"/>
-      <c r="H35" s="118"/>
-      <c r="I35" s="119"/>
-      <c r="J35" s="104" t="s">
+      <c r="C35" s="123"/>
+      <c r="D35" s="123"/>
+      <c r="E35" s="123"/>
+      <c r="F35" s="123"/>
+      <c r="G35" s="123"/>
+      <c r="H35" s="123"/>
+      <c r="I35" s="124"/>
+      <c r="J35" s="107" t="s">
         <v>78</v>
       </c>
     </row>
@@ -23920,7 +23920,7 @@
       <c r="I36" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="J36" s="106"/>
+      <c r="J36" s="108"/>
     </row>
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="26" t="s">
@@ -23962,17 +23962,17 @@
     <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="41"/>
-      <c r="B40" s="122" t="s">
+      <c r="B40" s="127" t="s">
         <v>69</v>
       </c>
-      <c r="C40" s="118"/>
-      <c r="D40" s="118"/>
-      <c r="E40" s="118"/>
-      <c r="F40" s="118"/>
-      <c r="G40" s="118"/>
-      <c r="H40" s="118"/>
-      <c r="I40" s="119"/>
-      <c r="J40" s="104" t="s">
+      <c r="C40" s="123"/>
+      <c r="D40" s="123"/>
+      <c r="E40" s="123"/>
+      <c r="F40" s="123"/>
+      <c r="G40" s="123"/>
+      <c r="H40" s="123"/>
+      <c r="I40" s="124"/>
+      <c r="J40" s="107" t="s">
         <v>81</v>
       </c>
     </row>
@@ -24004,7 +24004,7 @@
       <c r="I41" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="J41" s="106"/>
+      <c r="J41" s="108"/>
     </row>
     <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="26" t="s">
@@ -24045,13 +24045,13 @@
     </row>
     <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="122" t="s">
+      <c r="A45" s="127" t="s">
         <v>82</v>
       </c>
-      <c r="B45" s="118"/>
-      <c r="C45" s="118"/>
-      <c r="D45" s="118"/>
-      <c r="E45" s="119"/>
+      <c r="B45" s="123"/>
+      <c r="C45" s="123"/>
+      <c r="D45" s="123"/>
+      <c r="E45" s="124"/>
     </row>
     <row r="46" spans="1:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="26" t="s">
@@ -24229,10 +24229,10 @@
       <c r="A60" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B60" s="131">
+      <c r="B60" s="104">
         <v>55273.5</v>
       </c>
-      <c r="C60" s="131">
+      <c r="C60" s="104">
         <v>51499.5</v>
       </c>
     </row>
@@ -24271,10 +24271,10 @@
       <c r="A64" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B64" s="131">
+      <c r="B64" s="104">
         <v>42332.9</v>
       </c>
-      <c r="C64" s="131">
+      <c r="C64" s="104">
         <v>38376.9</v>
       </c>
     </row>
@@ -24337,10 +24337,10 @@
       <c r="A71" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B71" s="131">
+      <c r="B71" s="104">
         <v>53916.4</v>
       </c>
-      <c r="C71" s="131">
+      <c r="C71" s="104">
         <v>51499.5</v>
       </c>
     </row>
@@ -24379,10 +24379,10 @@
       <c r="A75" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B75" s="131">
+      <c r="B75" s="104">
         <v>42332.9</v>
       </c>
-      <c r="C75" s="131">
+      <c r="C75" s="104">
         <v>38376.9</v>
       </c>
     </row>
@@ -24417,14 +24417,14 @@
       </c>
     </row>
     <row r="80" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C80" s="122" t="s">
+      <c r="C80" s="127" t="s">
         <v>149</v>
       </c>
-      <c r="D80" s="119"/>
-      <c r="E80" s="122" t="s">
+      <c r="D80" s="124"/>
+      <c r="E80" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="F80" s="119"/>
+      <c r="F80" s="124"/>
     </row>
     <row r="81" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B81" s="26" t="s">
@@ -24588,17 +24588,17 @@
       <c r="A90" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="B90" s="122" t="s">
+      <c r="B90" s="127" t="s">
         <v>69</v>
       </c>
-      <c r="C90" s="118"/>
-      <c r="D90" s="118"/>
-      <c r="E90" s="118"/>
-      <c r="F90" s="118"/>
-      <c r="G90" s="118"/>
-      <c r="H90" s="118"/>
-      <c r="I90" s="119"/>
-      <c r="J90" s="104" t="s">
+      <c r="C90" s="123"/>
+      <c r="D90" s="123"/>
+      <c r="E90" s="123"/>
+      <c r="F90" s="123"/>
+      <c r="G90" s="123"/>
+      <c r="H90" s="123"/>
+      <c r="I90" s="124"/>
+      <c r="J90" s="107" t="s">
         <v>78</v>
       </c>
     </row>
@@ -24630,7 +24630,7 @@
       <c r="I91" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="J91" s="106"/>
+      <c r="J91" s="108"/>
     </row>
     <row r="92" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="26" t="s">
@@ -24672,17 +24672,17 @@
     <row r="94" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="95" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="41"/>
-      <c r="B95" s="122" t="s">
+      <c r="B95" s="127" t="s">
         <v>69</v>
       </c>
-      <c r="C95" s="118"/>
-      <c r="D95" s="118"/>
-      <c r="E95" s="118"/>
-      <c r="F95" s="118"/>
-      <c r="G95" s="118"/>
-      <c r="H95" s="118"/>
-      <c r="I95" s="119"/>
-      <c r="J95" s="104" t="s">
+      <c r="C95" s="123"/>
+      <c r="D95" s="123"/>
+      <c r="E95" s="123"/>
+      <c r="F95" s="123"/>
+      <c r="G95" s="123"/>
+      <c r="H95" s="123"/>
+      <c r="I95" s="124"/>
+      <c r="J95" s="107" t="s">
         <v>81</v>
       </c>
     </row>
@@ -24714,7 +24714,7 @@
       <c r="I96" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="J96" s="106"/>
+      <c r="J96" s="108"/>
     </row>
     <row r="97" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="26" t="s">
@@ -24755,13 +24755,13 @@
     </row>
     <row r="99" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="100" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="122" t="s">
+      <c r="A100" s="127" t="s">
         <v>82</v>
       </c>
-      <c r="B100" s="118"/>
-      <c r="C100" s="118"/>
-      <c r="D100" s="118"/>
-      <c r="E100" s="119"/>
+      <c r="B100" s="123"/>
+      <c r="C100" s="123"/>
+      <c r="D100" s="123"/>
+      <c r="E100" s="124"/>
     </row>
     <row r="101" spans="1:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="26" t="s">
@@ -24943,22 +24943,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="127" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="119"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="124"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="122" t="s">
+      <c r="A3" s="127" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="118"/>
-      <c r="C3" s="118"/>
-      <c r="D3" s="118"/>
-      <c r="E3" s="119"/>
+      <c r="B3" s="123"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="124"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="26"/>
@@ -25120,16 +25120,16 @@
       <c r="A14" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="132">
+      <c r="B14" s="105">
         <v>-1483.3</v>
       </c>
-      <c r="C14" s="132">
+      <c r="C14" s="105">
         <v>-6080.4</v>
       </c>
-      <c r="D14" s="132">
+      <c r="D14" s="105">
         <v>-170.2</v>
       </c>
-      <c r="E14" s="132">
+      <c r="E14" s="105">
         <v>-7733.9</v>
       </c>
     </row>
@@ -25261,16 +25261,16 @@
       <c r="A23" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="132">
+      <c r="B23" s="105">
         <v>243.3</v>
       </c>
-      <c r="C23" s="132">
+      <c r="C23" s="105">
         <v>-6139.9</v>
       </c>
-      <c r="D23" s="132">
+      <c r="D23" s="105">
         <v>166.2</v>
       </c>
-      <c r="E23" s="132">
+      <c r="E23" s="105">
         <v>-5730.4</v>
       </c>
     </row>
@@ -25295,16 +25295,16 @@
       <c r="A25" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="B25" s="133">
+      <c r="B25" s="106">
         <v>43170.1</v>
       </c>
-      <c r="C25" s="133">
+      <c r="C25" s="106">
         <v>270427.5</v>
       </c>
-      <c r="D25" s="133">
+      <c r="D25" s="106">
         <v>4793.3</v>
       </c>
-      <c r="E25" s="133">
+      <c r="E25" s="106">
         <v>318390.90000000002</v>
       </c>
     </row>
@@ -25327,13 +25327,13 @@
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="122" t="s">
+      <c r="A28" s="127" t="s">
         <v>176</v>
       </c>
-      <c r="B28" s="118"/>
-      <c r="C28" s="118"/>
-      <c r="D28" s="118"/>
-      <c r="E28" s="119"/>
+      <c r="B28" s="123"/>
+      <c r="C28" s="123"/>
+      <c r="D28" s="123"/>
+      <c r="E28" s="124"/>
     </row>
     <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="26"/>
@@ -25495,16 +25495,16 @@
       <c r="A39" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="132">
+      <c r="B39" s="105">
         <v>-1870</v>
       </c>
-      <c r="C39" s="132">
+      <c r="C39" s="105">
         <v>-9620.5</v>
       </c>
-      <c r="D39" s="132">
+      <c r="D39" s="105">
         <v>-238.6</v>
       </c>
-      <c r="E39" s="132">
+      <c r="E39" s="105">
         <v>-11729.1</v>
       </c>
     </row>
@@ -25636,16 +25636,16 @@
       <c r="A48" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B48" s="132">
+      <c r="B48" s="105">
         <v>256.5</v>
       </c>
-      <c r="C48" s="132">
+      <c r="C48" s="105">
         <v>-3421.5</v>
       </c>
-      <c r="D48" s="132">
+      <c r="D48" s="105">
         <v>172</v>
       </c>
-      <c r="E48" s="132">
+      <c r="E48" s="105">
         <v>-2993</v>
       </c>
     </row>
@@ -25670,16 +25670,16 @@
       <c r="A50" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="B50" s="131">
+      <c r="B50" s="104">
         <v>46368.6</v>
       </c>
-      <c r="C50" s="131">
+      <c r="C50" s="104">
         <v>211290.9</v>
       </c>
-      <c r="D50" s="131">
+      <c r="D50" s="104">
         <v>4101.3999999999996</v>
       </c>
-      <c r="E50" s="131">
+      <c r="E50" s="104">
         <v>261760.9</v>
       </c>
     </row>
@@ -25706,22 +25706,22 @@
       </c>
     </row>
     <row r="54" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="122" t="s">
+      <c r="A54" s="127" t="s">
         <v>95</v>
       </c>
-      <c r="B54" s="118"/>
-      <c r="C54" s="118"/>
-      <c r="D54" s="118"/>
-      <c r="E54" s="119"/>
+      <c r="B54" s="123"/>
+      <c r="C54" s="123"/>
+      <c r="D54" s="123"/>
+      <c r="E54" s="124"/>
     </row>
     <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="122" t="s">
+      <c r="A55" s="127" t="s">
         <v>96</v>
       </c>
-      <c r="B55" s="118"/>
-      <c r="C55" s="118"/>
-      <c r="D55" s="118"/>
-      <c r="E55" s="119"/>
+      <c r="B55" s="123"/>
+      <c r="C55" s="123"/>
+      <c r="D55" s="123"/>
+      <c r="E55" s="124"/>
     </row>
     <row r="56" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="26"/>
@@ -25883,16 +25883,16 @@
       <c r="A66" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="132">
+      <c r="B66" s="105">
         <v>1157.9000000000001</v>
       </c>
-      <c r="C66" s="132">
+      <c r="C66" s="105">
         <v>1998.9</v>
       </c>
-      <c r="D66" s="132" t="s">
-        <v>5</v>
-      </c>
-      <c r="E66" s="132">
+      <c r="D66" s="105" t="s">
+        <v>5</v>
+      </c>
+      <c r="E66" s="105">
         <v>3156.8</v>
       </c>
     </row>
@@ -26024,16 +26024,16 @@
       <c r="A75" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B75" s="132">
+      <c r="B75" s="105">
         <v>-18.7</v>
       </c>
-      <c r="C75" s="132">
+      <c r="C75" s="105">
         <v>-6343.6</v>
       </c>
-      <c r="D75" s="132" t="s">
-        <v>5</v>
-      </c>
-      <c r="E75" s="132">
+      <c r="D75" s="105" t="s">
+        <v>5</v>
+      </c>
+      <c r="E75" s="105">
         <v>-6362.3</v>
       </c>
     </row>
@@ -26058,16 +26058,16 @@
       <c r="A77" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="B77" s="131">
+      <c r="B77" s="104">
         <v>11962.9</v>
       </c>
-      <c r="C77" s="131">
+      <c r="C77" s="104">
         <v>48688.2</v>
       </c>
-      <c r="D77" s="131" t="s">
-        <v>5</v>
-      </c>
-      <c r="E77" s="131">
+      <c r="D77" s="104" t="s">
+        <v>5</v>
+      </c>
+      <c r="E77" s="104">
         <v>60651.1</v>
       </c>
     </row>
@@ -26090,13 +26090,13 @@
     </row>
     <row r="79" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="80" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="122" t="s">
+      <c r="A80" s="127" t="s">
         <v>176</v>
       </c>
-      <c r="B80" s="118"/>
-      <c r="C80" s="118"/>
-      <c r="D80" s="118"/>
-      <c r="E80" s="119"/>
+      <c r="B80" s="123"/>
+      <c r="C80" s="123"/>
+      <c r="D80" s="123"/>
+      <c r="E80" s="124"/>
     </row>
     <row r="81" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="26"/>
@@ -26258,16 +26258,16 @@
       <c r="A91" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B91" s="132">
+      <c r="B91" s="105">
         <v>1440.8</v>
       </c>
-      <c r="C91" s="132">
+      <c r="C91" s="105">
         <v>122.3</v>
       </c>
-      <c r="D91" s="132" t="s">
-        <v>5</v>
-      </c>
-      <c r="E91" s="132">
+      <c r="D91" s="105" t="s">
+        <v>5</v>
+      </c>
+      <c r="E91" s="105">
         <v>1563.1</v>
       </c>
     </row>
@@ -26399,16 +26399,16 @@
       <c r="A100" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B100" s="132">
+      <c r="B100" s="105">
         <v>-13.4</v>
       </c>
-      <c r="C100" s="132">
+      <c r="C100" s="105">
         <v>-4078.3</v>
       </c>
-      <c r="D100" s="132" t="s">
-        <v>5</v>
-      </c>
-      <c r="E100" s="132">
+      <c r="D100" s="105" t="s">
+        <v>5</v>
+      </c>
+      <c r="E100" s="105">
         <v>-4091.7</v>
       </c>
     </row>
@@ -26433,16 +26433,16 @@
       <c r="A102" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="B102" s="131">
+      <c r="B102" s="104">
         <v>13122.6</v>
       </c>
-      <c r="C102" s="131">
+      <c r="C102" s="104">
         <v>38376.9</v>
       </c>
-      <c r="D102" s="131" t="s">
-        <v>5</v>
-      </c>
-      <c r="E102" s="131">
+      <c r="D102" s="104" t="s">
+        <v>5</v>
+      </c>
+      <c r="E102" s="104">
         <v>51499.5</v>
       </c>
     </row>
@@ -26497,32 +26497,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="127" t="s">
         <v>231</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="118"/>
-      <c r="H1" s="118"/>
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
     </row>
     <row r="2" spans="1:8" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="123" t="s">
+      <c r="A2" s="128" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="124"/>
-      <c r="C2" s="125"/>
-      <c r="D2" s="126" t="s">
+      <c r="B2" s="129"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="131" t="s">
         <v>110</v>
       </c>
-      <c r="E2" s="127"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="126" t="s">
+      <c r="E2" s="132"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="131" t="s">
         <v>111</v>
       </c>
-      <c r="H2" s="128"/>
+      <c r="H2" s="133"/>
     </row>
     <row r="3" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="45" t="s">
@@ -26623,32 +26623,32 @@
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="122" t="s">
+      <c r="A11" s="127" t="s">
         <v>232</v>
       </c>
-      <c r="B11" s="118"/>
-      <c r="C11" s="118"/>
-      <c r="D11" s="118"/>
-      <c r="E11" s="118"/>
-      <c r="F11" s="118"/>
-      <c r="G11" s="118"/>
-      <c r="H11" s="118"/>
+      <c r="B11" s="123"/>
+      <c r="C11" s="123"/>
+      <c r="D11" s="123"/>
+      <c r="E11" s="123"/>
+      <c r="F11" s="123"/>
+      <c r="G11" s="123"/>
+      <c r="H11" s="123"/>
     </row>
     <row r="12" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="123" t="s">
+      <c r="A12" s="128" t="s">
         <v>109</v>
       </c>
-      <c r="B12" s="124"/>
-      <c r="C12" s="125"/>
-      <c r="D12" s="126" t="s">
+      <c r="B12" s="129"/>
+      <c r="C12" s="130"/>
+      <c r="D12" s="131" t="s">
         <v>110</v>
       </c>
-      <c r="E12" s="127"/>
-      <c r="F12" s="128"/>
-      <c r="G12" s="126" t="s">
+      <c r="E12" s="132"/>
+      <c r="F12" s="133"/>
+      <c r="G12" s="131" t="s">
         <v>111</v>
       </c>
-      <c r="H12" s="128"/>
+      <c r="H12" s="133"/>
     </row>
     <row r="13" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="45" t="s">
@@ -26751,32 +26751,32 @@
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="122" t="s">
+      <c r="A21" s="127" t="s">
         <v>233</v>
       </c>
-      <c r="B21" s="118"/>
-      <c r="C21" s="118"/>
-      <c r="D21" s="118"/>
-      <c r="E21" s="118"/>
-      <c r="F21" s="118"/>
-      <c r="G21" s="118"/>
-      <c r="H21" s="118"/>
+      <c r="B21" s="123"/>
+      <c r="C21" s="123"/>
+      <c r="D21" s="123"/>
+      <c r="E21" s="123"/>
+      <c r="F21" s="123"/>
+      <c r="G21" s="123"/>
+      <c r="H21" s="123"/>
     </row>
     <row r="22" spans="1:8" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="123" t="s">
+      <c r="A22" s="128" t="s">
         <v>109</v>
       </c>
-      <c r="B22" s="124"/>
-      <c r="C22" s="125"/>
-      <c r="D22" s="126" t="s">
+      <c r="B22" s="129"/>
+      <c r="C22" s="130"/>
+      <c r="D22" s="131" t="s">
         <v>110</v>
       </c>
-      <c r="E22" s="127"/>
-      <c r="F22" s="128"/>
-      <c r="G22" s="126" t="s">
+      <c r="E22" s="132"/>
+      <c r="F22" s="133"/>
+      <c r="G22" s="131" t="s">
         <v>111</v>
       </c>
-      <c r="H22" s="128"/>
+      <c r="H22" s="133"/>
     </row>
     <row r="23" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="45" t="s">
@@ -26877,32 +26877,32 @@
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="122" t="s">
+      <c r="A31" s="127" t="s">
         <v>242</v>
       </c>
-      <c r="B31" s="118"/>
-      <c r="C31" s="118"/>
-      <c r="D31" s="118"/>
-      <c r="E31" s="118"/>
-      <c r="F31" s="118"/>
-      <c r="G31" s="118"/>
-      <c r="H31" s="118"/>
+      <c r="B31" s="123"/>
+      <c r="C31" s="123"/>
+      <c r="D31" s="123"/>
+      <c r="E31" s="123"/>
+      <c r="F31" s="123"/>
+      <c r="G31" s="123"/>
+      <c r="H31" s="123"/>
     </row>
     <row r="32" spans="1:8" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="123" t="s">
+      <c r="A32" s="128" t="s">
         <v>109</v>
       </c>
-      <c r="B32" s="124"/>
-      <c r="C32" s="125"/>
-      <c r="D32" s="126" t="s">
+      <c r="B32" s="129"/>
+      <c r="C32" s="130"/>
+      <c r="D32" s="131" t="s">
         <v>110</v>
       </c>
-      <c r="E32" s="127"/>
-      <c r="F32" s="128"/>
-      <c r="G32" s="126" t="s">
+      <c r="E32" s="132"/>
+      <c r="F32" s="133"/>
+      <c r="G32" s="131" t="s">
         <v>111</v>
       </c>
-      <c r="H32" s="128"/>
+      <c r="H32" s="133"/>
     </row>
     <row r="33" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="45" t="s">
@@ -27003,32 +27003,32 @@
     </row>
     <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="122" t="s">
+      <c r="A41" s="127" t="s">
         <v>243</v>
       </c>
-      <c r="B41" s="118"/>
-      <c r="C41" s="118"/>
-      <c r="D41" s="118"/>
-      <c r="E41" s="118"/>
-      <c r="F41" s="118"/>
-      <c r="G41" s="118"/>
-      <c r="H41" s="118"/>
+      <c r="B41" s="123"/>
+      <c r="C41" s="123"/>
+      <c r="D41" s="123"/>
+      <c r="E41" s="123"/>
+      <c r="F41" s="123"/>
+      <c r="G41" s="123"/>
+      <c r="H41" s="123"/>
     </row>
     <row r="42" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="123" t="s">
+      <c r="A42" s="128" t="s">
         <v>109</v>
       </c>
-      <c r="B42" s="124"/>
-      <c r="C42" s="125"/>
-      <c r="D42" s="126" t="s">
+      <c r="B42" s="129"/>
+      <c r="C42" s="130"/>
+      <c r="D42" s="131" t="s">
         <v>110</v>
       </c>
-      <c r="E42" s="127"/>
-      <c r="F42" s="128"/>
-      <c r="G42" s="126" t="s">
+      <c r="E42" s="132"/>
+      <c r="F42" s="133"/>
+      <c r="G42" s="131" t="s">
         <v>111</v>
       </c>
-      <c r="H42" s="128"/>
+      <c r="H42" s="133"/>
     </row>
     <row r="43" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="45" t="s">
@@ -27129,32 +27129,32 @@
     </row>
     <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="122" t="s">
+      <c r="A51" s="127" t="s">
         <v>244</v>
       </c>
-      <c r="B51" s="118"/>
-      <c r="C51" s="118"/>
-      <c r="D51" s="118"/>
-      <c r="E51" s="118"/>
-      <c r="F51" s="118"/>
-      <c r="G51" s="118"/>
-      <c r="H51" s="118"/>
+      <c r="B51" s="123"/>
+      <c r="C51" s="123"/>
+      <c r="D51" s="123"/>
+      <c r="E51" s="123"/>
+      <c r="F51" s="123"/>
+      <c r="G51" s="123"/>
+      <c r="H51" s="123"/>
     </row>
     <row r="52" spans="1:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="123" t="s">
+      <c r="A52" s="128" t="s">
         <v>109</v>
       </c>
-      <c r="B52" s="124"/>
-      <c r="C52" s="125"/>
-      <c r="D52" s="126" t="s">
+      <c r="B52" s="129"/>
+      <c r="C52" s="130"/>
+      <c r="D52" s="131" t="s">
         <v>110</v>
       </c>
-      <c r="E52" s="127"/>
-      <c r="F52" s="128"/>
-      <c r="G52" s="126" t="s">
+      <c r="E52" s="132"/>
+      <c r="F52" s="133"/>
+      <c r="G52" s="131" t="s">
         <v>111</v>
       </c>
-      <c r="H52" s="128"/>
+      <c r="H52" s="133"/>
     </row>
     <row r="53" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="45" t="s">
@@ -27259,6 +27259,14 @@
     <row r="72" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A51:H51"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="D52:F52"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="G42:H42"/>
     <mergeCell ref="A41:H41"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:F2"/>
@@ -27275,14 +27283,6 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="G12:H12"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A51:H51"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="D52:F52"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="G42:H42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -27382,12 +27382,12 @@
       <c r="A6" s="52"/>
     </row>
     <row r="7" spans="1:5" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="122" t="s">
+      <c r="A7" s="127" t="s">
         <v>122</v>
       </c>
-      <c r="B7" s="118"/>
-      <c r="C7" s="118"/>
-      <c r="D7" s="119"/>
+      <c r="B7" s="123"/>
+      <c r="C7" s="123"/>
+      <c r="D7" s="124"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="45" t="s">
@@ -27522,12 +27522,12 @@
       <c r="A18" s="52"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="122" t="s">
+      <c r="A19" s="127" t="s">
         <v>122</v>
       </c>
-      <c r="B19" s="118"/>
-      <c r="C19" s="118"/>
-      <c r="D19" s="119"/>
+      <c r="B19" s="123"/>
+      <c r="C19" s="123"/>
+      <c r="D19" s="124"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="45" t="s">
@@ -27598,7 +27598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -27616,11 +27616,11 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="127" t="s">
         <v>181</v>
       </c>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="123"/>
     </row>
     <row r="3" spans="1:5" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
@@ -27723,14 +27723,14 @@
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:5" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="122" t="s">
+      <c r="B13" s="127" t="s">
         <v>183</v>
       </c>
-      <c r="C13" s="119"/>
-      <c r="D13" s="122" t="s">
+      <c r="C13" s="124"/>
+      <c r="D13" s="127" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="119"/>
+      <c r="E13" s="124"/>
     </row>
     <row r="14" spans="1:5" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="47" t="s">

</xml_diff>